<commit_message>
"Deleted extra workflows and Zip Code Validation is in Progress. "
</commit_message>
<xml_diff>
--- a/PinCode.xlsx
+++ b/PinCode.xlsx
@@ -14,21 +14,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <x:si>
     <x:t>744105</x:t>
-  </x:si>
-  <x:si>
-    <x:t>744207</x:t>
-  </x:si>
-  <x:si>
-    <x:t>744106</x:t>
-  </x:si>
-  <x:si>
-    <x:t>744103</x:t>
-  </x:si>
-  <x:si>
-    <x:t>110026</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -379,7 +367,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:A5"/>
+  <x:dimension ref="A1:A1"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -390,26 +378,6 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="2" spans="1:1">
-      <x:c r="A2" s="0" t="s">
-        <x:v>1</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="3" spans="1:1">
-      <x:c r="A3" s="0" t="s">
-        <x:v>2</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="4" spans="1:1">
-      <x:c r="A4" s="0" t="s">
-        <x:v>3</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="5" spans="1:1">
-      <x:c r="A5" s="0" t="s">
-        <x:v>4</x:v>
-      </x:c>
-    </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>